<commit_message>
Removed MMS for children intervention
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2017Sep/InputForCode_Tanzania14Sep17.xlsx
+++ b/input_spreadsheets/Tanzania/2017Sep/InputForCode_Tanzania14Sep17.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/2017Sep/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -108,33 +108,10 @@
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author xml:space="preserve"> Janka Petravic</author>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Sprinkles, acts the same as vitamin A if we ignore the effect on anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E6" authorId="1">
+    <comment ref="E4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -163,33 +140,10 @@
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author xml:space="preserve"> Janka Petravic</author>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Sprinkles, acts the same as vitamin A if we ignore the effect on anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E6" authorId="1">
+    <comment ref="E4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -362,6 +316,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author xml:space="preserve"> Janka Petravic</author>
+    <author>Sam</author>
   </authors>
   <commentList>
     <comment ref="A2" authorId="0">
@@ -383,6 +338,28 @@
           </rPr>
           <t xml:space="preserve">
 LiST has higher values 'recalculated across countries for consistency'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+All 'normal' and 'mild' categories are fictional</t>
         </r>
       </text>
     </comment>
@@ -918,33 +895,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Sprinkles, acts the same as vitamin A if we ignore the effect on anemia</t>
+Cochrane review - not finished; no who guidelines.</t>
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Cochrane review - not finished; no who guidelines.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D9" authorId="0">
+    <comment ref="D8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1065,72 +1020,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Sprinkles</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D8" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Constrained by vitamin A supplementation</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E8" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Constrained by vitamin A supplementation</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -1217,51 +1106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Sprinkles, acts the same as vitamin A if we ignore the effect on anemia</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="E4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic: 
-fraction</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> vitamin A deficient</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1288,7 +1133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="81">
   <si>
     <t>indicators</t>
   </si>
@@ -1528,9 +1373,6 @@
   </si>
   <si>
     <t>Antenatal micronutrient supplementation</t>
-  </si>
-  <si>
-    <t>Multiple micronutrients for children</t>
   </si>
   <si>
     <t>Vitamin A fortification of food</t>
@@ -1737,7 +1579,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1781,32 +1623,23 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="57">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -1994,8 +1827,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2045,8 +1878,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2096,8 +1929,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2147,8 +1980,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2198,8 +2031,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2249,8 +2082,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2300,8 +2133,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2351,8 +2184,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2402,8 +2235,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2453,8 +2286,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2504,8 +2337,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2555,8 +2388,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2606,8 +2439,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2657,8 +2490,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2708,8 +2541,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2759,8 +2592,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2810,8 +2643,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2861,8 +2694,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -2912,8 +2745,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -3283,7 +3116,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5019,10 +4852,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5051,13 +4884,13 @@
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="24">
         <v>0.89970000000000006</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="24">
         <v>0.95</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="24">
         <v>0.4</v>
       </c>
       <c r="E2" s="5"/>
@@ -5068,13 +4901,13 @@
       <c r="A3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="32">
+      <c r="B3" s="24">
         <v>0.19939999999999999</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="24">
         <v>0.95</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="24">
         <v>11.19</v>
       </c>
       <c r="E3" s="5"/>
@@ -5091,7 +4924,7 @@
       <c r="C4" s="5">
         <v>0.95</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="25">
         <v>48</v>
       </c>
       <c r="E4" s="5"/>
@@ -5102,13 +4935,13 @@
       <c r="A5" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="24">
         <v>0.23080000000000001</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="24">
         <v>0.95</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="24">
         <v>26.05</v>
       </c>
       <c r="E5" s="5"/>
@@ -5125,7 +4958,7 @@
       <c r="C6" s="5">
         <v>0.95</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="25">
         <v>25</v>
       </c>
     </row>
@@ -5133,13 +4966,13 @@
       <c r="A7" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="24">
         <v>0.3538</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="24">
         <v>0.95</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="24">
         <v>3.42</v>
       </c>
       <c r="E7" s="5"/>
@@ -5150,37 +4983,27 @@
       <c r="A8" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="32">
-        <v>0.1</v>
-      </c>
-      <c r="C8" s="34">
+      <c r="B8" s="24">
+        <v>0</v>
+      </c>
+      <c r="C8" s="26">
         <v>0.95</v>
       </c>
-      <c r="D8" s="32">
-        <v>5.43</v>
+      <c r="D8" s="24">
+        <v>0.32</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="32">
-        <v>0</v>
-      </c>
-      <c r="C9" s="34">
-        <v>0.95</v>
-      </c>
-      <c r="D9" s="32">
-        <v>0.32</v>
-      </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -5201,10 +5024,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="5"/>
@@ -5249,10 +5069,6 @@
     <row r="24" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5263,10 +5079,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5462,34 +5278,18 @@
         <v>1</v>
       </c>
       <c r="F8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
+      <c r="B9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="5"/>
@@ -5507,10 +5307,7 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
@@ -5555,10 +5352,6 @@
     <row r="23" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5678,15 +5471,15 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="16"/>
     </row>
   </sheetData>
@@ -5698,10 +5491,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:G7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5799,7 +5592,6 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -5816,49 +5608,6 @@
         <v>0</v>
       </c>
       <c r="G5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.41599999999999998</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0.41599999999999998</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0.41599999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5871,10 +5620,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:G7"/>
+      <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5961,18 +5710,20 @@
       <c r="D4" s="5">
         <v>0</v>
       </c>
-      <c r="E4" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0.3</v>
+      <c r="E4" s="25">
+        <f>E2*0.8</f>
+        <v>0.24</v>
+      </c>
+      <c r="F4" s="25">
+        <f t="shared" ref="F4:G4" si="0">F2*0.8</f>
+        <v>0.24</v>
+      </c>
+      <c r="G4" s="25">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -5989,52 +5740,6 @@
         <v>0</v>
       </c>
       <c r="G5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="33">
-        <f>E2*0.8</f>
-        <v>0.24</v>
-      </c>
-      <c r="F6" s="33">
-        <f t="shared" ref="F6:G6" si="0">F2*0.8</f>
-        <v>0.24</v>
-      </c>
-      <c r="G6" s="33">
-        <f t="shared" si="0"/>
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -6047,10 +5752,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6137,18 +5842,20 @@
       <c r="D4" s="5">
         <v>0</v>
       </c>
-      <c r="E4" s="5">
-        <v>0.62</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.62</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0.62</v>
+      <c r="E4" s="25">
+        <f>E2*0.8</f>
+        <v>0.496</v>
+      </c>
+      <c r="F4" s="25">
+        <f t="shared" ref="F4:G4" si="0">F2*0.8</f>
+        <v>0.496</v>
+      </c>
+      <c r="G4" s="25">
+        <f t="shared" si="0"/>
+        <v>0.496</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -6165,52 +5872,6 @@
         <v>0</v>
       </c>
       <c r="G5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="33">
-        <f>E2*0.8</f>
-        <v>0.496</v>
-      </c>
-      <c r="F6" s="33">
-        <f t="shared" ref="F6:G6" si="0">F2*0.8</f>
-        <v>0.496</v>
-      </c>
-      <c r="G6" s="33">
-        <f t="shared" si="0"/>
-        <v>0.496</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -6648,7 +6309,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6683,60 +6344,80 @@
       <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
+      <c r="C2" s="27">
+        <v>43.35</v>
+      </c>
+      <c r="D2" s="27">
+        <v>43.35</v>
+      </c>
+      <c r="E2" s="27">
+        <v>40.270000000000003</v>
+      </c>
+      <c r="F2" s="27">
+        <v>30.974999999999998</v>
+      </c>
+      <c r="G2" s="27">
+        <v>30.314999999999998</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
+      <c r="C3" s="27">
+        <v>43.35</v>
+      </c>
+      <c r="D3" s="27">
+        <v>43.35</v>
+      </c>
+      <c r="E3" s="27">
+        <v>40.270000000000003</v>
+      </c>
+      <c r="F3" s="27">
+        <v>30.974999999999998</v>
+      </c>
+      <c r="G3" s="27">
+        <v>30.314999999999998</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="24">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="D4" s="24">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="E4" s="24">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="F4" s="24">
-        <v>0.2475</v>
-      </c>
-      <c r="G4" s="24">
-        <v>0.25940000000000002</v>
+      <c r="C4" s="27">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D4" s="27">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E4" s="27">
+        <v>13.700000000000001</v>
+      </c>
+      <c r="F4" s="27">
+        <v>24.75</v>
+      </c>
+      <c r="G4" s="27">
+        <v>25.94</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="24">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="D5" s="24">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="E5" s="24">
-        <v>5.7599999999999998E-2</v>
-      </c>
-      <c r="F5" s="24">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="G5" s="24">
-        <v>0.1343</v>
+      <c r="C5" s="27">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D5" s="27">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E5" s="27">
+        <v>5.76</v>
+      </c>
+      <c r="F5" s="27">
+        <v>13.3</v>
+      </c>
+      <c r="G5" s="27">
+        <v>13.43</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6746,60 +6427,80 @@
       <c r="B6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
+      <c r="C6" s="28">
+        <v>45.300000000000004</v>
+      </c>
+      <c r="D6" s="28">
+        <v>45.300000000000004</v>
+      </c>
+      <c r="E6" s="28">
+        <v>46.424999999999997</v>
+      </c>
+      <c r="F6" s="28">
+        <v>47.375</v>
+      </c>
+      <c r="G6" s="28">
+        <v>48.515000000000001</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="C7" s="28">
+        <v>45.300000000000004</v>
+      </c>
+      <c r="D7" s="28">
+        <v>45.300000000000004</v>
+      </c>
+      <c r="E7" s="28">
+        <v>46.424999999999997</v>
+      </c>
+      <c r="F7" s="28">
+        <v>47.375</v>
+      </c>
+      <c r="G7" s="28">
+        <v>48.515000000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="25">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="D8" s="25">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="E8" s="25">
-        <v>5.5500000000000001E-2</v>
-      </c>
-      <c r="F8" s="25">
-        <v>4.2500000000000003E-2</v>
-      </c>
-      <c r="G8" s="25">
-        <v>2.24E-2</v>
+      <c r="C8" s="28">
+        <v>5.4</v>
+      </c>
+      <c r="D8" s="28">
+        <v>5.4</v>
+      </c>
+      <c r="E8" s="28">
+        <v>5.55</v>
+      </c>
+      <c r="F8" s="28">
+        <v>4.25</v>
+      </c>
+      <c r="G8" s="28">
+        <v>2.2399999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="25">
-        <v>0.04</v>
-      </c>
-      <c r="D9" s="25">
-        <v>0.04</v>
-      </c>
-      <c r="E9" s="25">
-        <v>1.6E-2</v>
-      </c>
-      <c r="F9" s="25">
-        <v>0.01</v>
-      </c>
-      <c r="G9" s="25">
-        <v>7.3000000000000001E-3</v>
+      <c r="C9" s="28">
+        <v>4</v>
+      </c>
+      <c r="D9" s="28">
+        <v>4</v>
+      </c>
+      <c r="E9" s="28">
+        <v>1.6</v>
+      </c>
+      <c r="F9" s="28">
+        <v>1</v>
+      </c>
+      <c r="G9" s="28">
+        <v>0.73</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6809,19 +6510,19 @@
       <c r="B10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="28">
-        <v>0.84</v>
-      </c>
-      <c r="D10" s="29">
-        <v>0.50960000000000005</v>
-      </c>
-      <c r="E10" s="28">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F10" s="26">
-        <v>0</v>
-      </c>
-      <c r="G10" s="27">
+      <c r="C10" s="29">
+        <v>84</v>
+      </c>
+      <c r="D10" s="30">
+        <v>50.960000000000008</v>
+      </c>
+      <c r="E10" s="29">
+        <v>1.5</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8">
         <v>0</v>
       </c>
     </row>
@@ -6829,19 +6530,19 @@
       <c r="B11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="28">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="D11" s="29">
-        <v>0.19079999999999997</v>
-      </c>
-      <c r="E11" s="28">
-        <v>3.2500000000000001E-2</v>
-      </c>
-      <c r="F11" s="26">
-        <v>1E-3</v>
-      </c>
-      <c r="G11" s="27">
+      <c r="C11" s="29">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D11" s="30">
+        <v>19.079999999999998</v>
+      </c>
+      <c r="E11" s="29">
+        <v>3.25</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="G11" s="8">
         <v>0</v>
       </c>
     </row>
@@ -6849,19 +6550,19 @@
       <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="28">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="D12" s="30">
-        <v>0.27839999999999998</v>
-      </c>
-      <c r="E12" s="28">
-        <v>0.9355</v>
-      </c>
-      <c r="F12" s="26">
-        <v>0.72099999999999997</v>
-      </c>
-      <c r="G12" s="27">
+      <c r="C12" s="29">
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="D12" s="31">
+        <v>27.839999999999996</v>
+      </c>
+      <c r="E12" s="29">
+        <v>93.55</v>
+      </c>
+      <c r="F12" s="8">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="G12" s="8">
         <v>0</v>
       </c>
     </row>
@@ -6869,21 +6570,20 @@
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="28">
-        <v>0.01</v>
-      </c>
-      <c r="D13" s="30">
-        <v>2.12E-2</v>
-      </c>
-      <c r="E13" s="28">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="F13" s="26">
-        <f>1-F12-F11-F10</f>
-        <v>0.27800000000000002</v>
-      </c>
-      <c r="G13" s="27">
-        <v>1</v>
+      <c r="C13" s="29">
+        <v>1</v>
+      </c>
+      <c r="D13" s="31">
+        <v>2.12</v>
+      </c>
+      <c r="E13" s="29">
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="F13" s="8">
+        <v>27.800000000000004</v>
+      </c>
+      <c r="G13" s="8">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated stunting distribution to use normal distribution in spreadsheet
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2017Sep/InputForCode_Tanzania14Sep17.xlsx
+++ b/input_spreadsheets/Tanzania/2017Sep/InputForCode_Tanzania14Sep17.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="15" activeTab="24"/>
+    <workbookView xWindow="-38340" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -5754,7 +5754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
@@ -6308,8 +6308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6345,19 +6345,24 @@
         <v>20</v>
       </c>
       <c r="C2" s="27">
-        <v>43.35</v>
+        <f>(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5)/100, 0, 1) + 1, 0, 1, TRUE)) * 100</f>
+        <v>54.471569980476652</v>
       </c>
       <c r="D2" s="27">
-        <v>43.35</v>
+        <f t="shared" ref="D2:G2" si="0">(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5)/100, 0, 1) + 1, 0, 1, TRUE)) * 100</f>
+        <v>54.471569980476652</v>
       </c>
       <c r="E2" s="27">
-        <v>40.270000000000003</v>
+        <f t="shared" si="0"/>
+        <v>44.475236686630382</v>
       </c>
       <c r="F2" s="27">
-        <v>30.974999999999998</v>
+        <f t="shared" si="0"/>
+        <v>24.326698333409567</v>
       </c>
       <c r="G2" s="27">
-        <v>30.314999999999998</v>
+        <f t="shared" si="0"/>
+        <v>23.259986385548594</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6365,19 +6370,24 @@
         <v>29</v>
       </c>
       <c r="C3" s="27">
-        <v>43.35</v>
+        <f xml:space="preserve"> _xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5)/100,0,1)+1, 0, 1, TRUE)*100 - _xlfn.SUM(C4:C5)</f>
+        <v>32.228430019523351</v>
       </c>
       <c r="D3" s="27">
-        <v>43.35</v>
+        <f t="shared" ref="D3:G3" si="1" xml:space="preserve"> _xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5)/100,0,1)+1, 0, 1, TRUE)*100 - _xlfn.SUM(D4:D5)</f>
+        <v>32.228430019523351</v>
       </c>
       <c r="E3" s="27">
-        <v>40.270000000000003</v>
+        <f t="shared" si="1"/>
+        <v>36.064763313369617</v>
       </c>
       <c r="F3" s="27">
-        <v>30.974999999999998</v>
+        <f t="shared" si="1"/>
+        <v>37.623301666590436</v>
       </c>
       <c r="G3" s="27">
-        <v>30.314999999999998</v>
+        <f t="shared" si="1"/>
+        <v>37.370013614451409</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>